<commit_message>
added stats, and new card
</commit_message>
<xml_diff>
--- a/tactile_tabletop/Character Cards/Tactile_Tabletop_Data-Level_2_CC.xlsx
+++ b/tactile_tabletop/Character Cards/Tactile_Tabletop_Data-Level_2_CC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TableTopRolePlaying_Squib\tactile_tabletop\Character Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C46892-3F1E-49FB-B7C2-8B7B5AEF9065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7710CB86-D24D-4861-94B2-2A9729C1E7D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="292" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="292" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tactile Tabletop Data - Level 2" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="375">
   <si>
     <t>Top Ability Name</t>
   </si>
@@ -688,9 +688,6 @@
     <t>cha</t>
   </si>
   <si>
-    <t>per 8</t>
-  </si>
-  <si>
     <t>Robin</t>
   </si>
   <si>
@@ -700,9 +697,6 @@
     <t>kno</t>
   </si>
   <si>
-    <t>cha 15</t>
-  </si>
-  <si>
     <t>control sound in area</t>
   </si>
   <si>
@@ -736,9 +730,6 @@
     <t>spi</t>
   </si>
   <si>
-    <t>fin 22</t>
-  </si>
-  <si>
     <t>prevent overstep</t>
   </si>
   <si>
@@ -1025,6 +1016,138 @@
   </si>
   <si>
     <t>2 Level Points</t>
+  </si>
+  <si>
+    <t>Kno 4</t>
+  </si>
+  <si>
+    <t>Vig 4</t>
+  </si>
+  <si>
+    <t>Cha 4</t>
+  </si>
+  <si>
+    <t>Str 2, Kno 1, Fin 1</t>
+  </si>
+  <si>
+    <t>Cra 3, Fin 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kno 2, Spi 1, Kno 1 </t>
+  </si>
+  <si>
+    <t>Fin 4</t>
+  </si>
+  <si>
+    <t>Str 3, Cha 1</t>
+  </si>
+  <si>
+    <t>Cra 2, Fin 2</t>
+  </si>
+  <si>
+    <t>Vig 2, Str 1, Cha 1</t>
+  </si>
+  <si>
+    <t>Per 4</t>
+  </si>
+  <si>
+    <t>Vig 2, Per 2</t>
+  </si>
+  <si>
+    <t>Vig 2, Str 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spi 3, Kno 1 </t>
+  </si>
+  <si>
+    <t>Cra 2, Fin 1, Spi 1</t>
+  </si>
+  <si>
+    <t>Str 2, Cra 1, Fin 1</t>
+  </si>
+  <si>
+    <t>Fin 2, Str 2</t>
+  </si>
+  <si>
+    <t>Cha 2, Cra 2</t>
+  </si>
+  <si>
+    <t>Spi 2, Vig 1, Per 1</t>
+  </si>
+  <si>
+    <t>Per 2, Cha 1, Fin 1</t>
+  </si>
+  <si>
+    <t>Cha 2, Str 1, Kno 1</t>
+  </si>
+  <si>
+    <t>Fin 2, Str 1, Cha 1</t>
+  </si>
+  <si>
+    <t>Spi 2, Cha 2</t>
+  </si>
+  <si>
+    <t>Kno 2, Str 1, Fin 1</t>
+  </si>
+  <si>
+    <t>Per 3, Str 1</t>
+  </si>
+  <si>
+    <t>Spi 3, Fin 1</t>
+  </si>
+  <si>
+    <t>Spi 4</t>
+  </si>
+  <si>
+    <t>Kno 2, Cha 2</t>
+  </si>
+  <si>
+    <t>Str 2, Vig 2</t>
+  </si>
+  <si>
+    <t>Str 4</t>
+  </si>
+  <si>
+    <t>Vig 3, Kno 1</t>
+  </si>
+  <si>
+    <t>Spi 2, Cra 1, Fin 1</t>
+  </si>
+  <si>
+    <t>Cha 3, Fin 1</t>
+  </si>
+  <si>
+    <t>Cra 4</t>
+  </si>
+  <si>
+    <t>Cha 1, Fin 3</t>
+  </si>
+  <si>
+    <t>Kno 2, Spi 2</t>
+  </si>
+  <si>
+    <t>per, fin</t>
+  </si>
+  <si>
+    <t>Gain movement ; mark usage (for more movement)</t>
+  </si>
+  <si>
+    <t>beat influence ; debuff enemy movement ; mark usage</t>
+  </si>
+  <si>
+    <t>per, cha</t>
+  </si>
+  <si>
+    <t>Per 2, Fin 1, Cha 1</t>
+  </si>
+  <si>
+    <t>per 10</t>
+  </si>
+  <si>
+    <t>fin 23</t>
+  </si>
+  <si>
+    <t>cha 16</t>
   </si>
 </sst>
 </file>
@@ -1512,7 +1635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="P41" sqref="P41"/>
     </sheetView>
   </sheetViews>
@@ -1531,9 +1654,10 @@
     <col min="13" max="13" width="33" style="1" customWidth="1"/>
     <col min="14" max="14" width="8.7109375" style="1" customWidth="1"/>
     <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="16.85546875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="53.42578125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="6.5703125" style="1"/>
+    <col min="16" max="16" width="17.7109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="11" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="6.5703125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="63.75" x14ac:dyDescent="0.2">
@@ -1633,7 +1757,10 @@
         <v>30</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
@@ -1674,7 +1801,10 @@
         <v>30</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
@@ -1718,7 +1848,10 @@
         <v>23</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
@@ -1762,6 +1895,9 @@
         <v>23</v>
       </c>
       <c r="O5" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>333</v>
       </c>
     </row>
@@ -1809,7 +1945,10 @@
         <v>30</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="89.25" x14ac:dyDescent="0.2">
@@ -1856,7 +1995,10 @@
         <v>23</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="51" x14ac:dyDescent="0.2">
@@ -1900,7 +2042,10 @@
         <v>30</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="51" x14ac:dyDescent="0.2">
@@ -1947,7 +2092,10 @@
         <v>30</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="51" x14ac:dyDescent="0.2">
@@ -1994,7 +2142,10 @@
         <v>74</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="76.5" x14ac:dyDescent="0.2">
@@ -2041,7 +2192,10 @@
         <v>23</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="63.75" x14ac:dyDescent="0.2">
@@ -2088,7 +2242,10 @@
         <v>74</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="51" x14ac:dyDescent="0.2">
@@ -2135,7 +2292,10 @@
         <v>23</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
@@ -2179,7 +2339,10 @@
         <v>30</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
@@ -2226,7 +2389,10 @@
         <v>30</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
@@ -2273,10 +2439,13 @@
         <v>30</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>108</v>
       </c>
@@ -2320,10 +2489,13 @@
         <v>30</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>112</v>
       </c>
@@ -2367,10 +2539,13 @@
         <v>30</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>330</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>116</v>
       </c>
@@ -2414,10 +2589,13 @@
         <v>23</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="63.75" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>120</v>
       </c>
@@ -2461,10 +2639,13 @@
         <v>23</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+        <v>330</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>126</v>
       </c>
@@ -2505,10 +2686,13 @@
         <v>30</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>130</v>
       </c>
@@ -2552,10 +2736,13 @@
         <v>23</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>135</v>
       </c>
@@ -2599,10 +2786,13 @@
         <v>30</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>140</v>
       </c>
@@ -2640,10 +2830,13 @@
         <v>30</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>144</v>
       </c>
@@ -2687,10 +2880,13 @@
         <v>23</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="63.75" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>148</v>
       </c>
@@ -2731,10 +2927,13 @@
         <v>30</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>152</v>
       </c>
@@ -2778,10 +2977,13 @@
         <v>30</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>156</v>
       </c>
@@ -2825,10 +3027,13 @@
         <v>30</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="76.5" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>160</v>
       </c>
@@ -2872,10 +3077,13 @@
         <v>30</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>165</v>
       </c>
@@ -2916,10 +3124,13 @@
         <v>23</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>171</v>
       </c>
@@ -2960,10 +3171,13 @@
         <v>23</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>175</v>
       </c>
@@ -2980,7 +3194,7 @@
         <v>21</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>23</v>
@@ -2995,22 +3209,25 @@
         <v>55</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>21</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="N32" s="1" t="s">
         <v>23</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" ht="102" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>177</v>
       </c>
@@ -3042,7 +3259,7 @@
         <v>55</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>21</v>
@@ -3054,10 +3271,13 @@
         <v>23</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>181</v>
       </c>
@@ -3098,10 +3318,13 @@
         <v>30</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>185</v>
       </c>
@@ -3112,7 +3335,7 @@
         <v>55</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>38</v>
@@ -3145,10 +3368,13 @@
         <v>30</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>189</v>
       </c>
@@ -3192,10 +3418,13 @@
         <v>23</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" ht="76.5" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>193</v>
       </c>
@@ -3239,10 +3468,13 @@
         <v>23</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" ht="63.75" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>197</v>
       </c>
@@ -3283,10 +3515,13 @@
         <v>23</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" ht="63.75" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="P38" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>203</v>
       </c>
@@ -3327,10 +3562,13 @@
         <v>23</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>207</v>
       </c>
@@ -3371,12 +3609,15 @@
         <v>23</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>37</v>
@@ -3388,13 +3629,13 @@
         <v>28</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>25</v>
@@ -3409,13 +3650,16 @@
         <v>44</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="N41" s="1" t="s">
         <v>23</v>
       </c>
       <c r="O41" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>371</v>
       </c>
     </row>
   </sheetData>
@@ -3429,10 +3673,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H79"/>
+  <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3511,13 +3755,13 @@
         <v>220</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>221</v>
+        <v>372</v>
       </c>
       <c r="G4">
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -3528,13 +3772,13 @@
         <v>37</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>224</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>225</v>
+        <v>374</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -3551,19 +3795,19 @@
         <v>64</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>228</v>
       </c>
       <c r="G6">
         <v>2</v>
       </c>
       <c r="H6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -3574,19 +3818,19 @@
         <v>200</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -3600,13 +3844,13 @@
         <v>49</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>232</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>234</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -3623,13 +3867,13 @@
         <v>64</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>237</v>
+        <v>373</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -3643,19 +3887,19 @@
         <v>25</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>220</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -3666,19 +3910,19 @@
         <v>25</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="G11">
         <v>2</v>
       </c>
       <c r="H11" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -3690,316 +3934,317 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>114</v>
+        <v>326</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>245</v>
+        <v>368</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>246</v>
-      </c>
+        <v>367</v>
+      </c>
+      <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>187</v>
+        <v>114</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>64</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>156</v>
+        <v>187</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>236</v>
+        <v>247</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>64</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>254</v>
+        <v>223</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>51</v>
+        <v>181</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>233</v>
+        <v>253</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>259</v>
+        <v>231</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>120</v>
+        <v>17</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>121</v>
+        <v>18</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>233</v>
+        <v>256</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>18</v>
+        <v>121</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>106</v>
+        <v>49</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>169</v>
+        <v>105</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>48</v>
+        <v>177</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>25</v>
+        <v>121</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>175</v>
+        <v>48</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>124</v>
+        <v>49</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>265</v>
+        <v>231</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>266</v>
+        <v>124</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>233</v>
+        <v>261</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>270</v>
+        <v>264</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>148</v>
+        <v>176</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>124</v>
+        <v>265</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>25</v>
@@ -4008,336 +4253,336 @@
         <v>124</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="B33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="D33" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" s="1" t="s">
+      <c r="B34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>277</v>
+      <c r="D34" s="3" t="s">
+        <v>273</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>248</v>
+        <v>267</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>54</v>
+        <v>123</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>56</v>
+        <v>124</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>227</v>
+        <v>245</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>133</v>
+        <v>54</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>185</v>
+        <v>133</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>280</v>
+        <v>41</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>248</v>
+        <v>225</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>64</v>
+        <v>277</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>75</v>
+        <v>189</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="D43" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B44" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="F43" s="3"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>286</v>
-      </c>
+      <c r="D44" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="F44" s="3"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>103</v>
+        <v>37</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>165</v>
+        <v>102</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>167</v>
+        <v>103</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="E47" s="1" t="s">
+      <c r="D48" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="E48" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>220</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>130</v>
+        <v>195</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>220</v>
+        <v>288</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>25</v>
@@ -4346,7 +4591,7 @@
         <v>44</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>220</v>
@@ -4354,7 +4599,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>203</v>
+        <v>146</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>25</v>
@@ -4363,49 +4608,49 @@
         <v>44</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>295</v>
+        <v>220</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>24</v>
+        <v>203</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>244</v>
+        <v>292</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>25</v>
@@ -4414,50 +4659,50 @@
         <v>44</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B57" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C57" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D56" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="F56" s="3"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>244</v>
-      </c>
+      <c r="D57" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="F57" s="3"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>43</v>
+        <v>205</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>25</v>
@@ -4466,148 +4711,148 @@
         <v>44</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>220</v>
+        <v>241</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>99</v>
+        <v>43</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>100</v>
+        <v>44</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>303</v>
+        <v>217</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>217</v>
+        <v>300</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>140</v>
+        <v>328</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>305</v>
+        <v>369</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>217</v>
+        <v>370</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>286</v>
+        <v>217</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>138</v>
+        <v>37</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>108</v>
+        <v>34</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>309</v>
+        <v>64</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>303</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>236</v>
+        <v>283</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>92</v>
+        <v>25</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>41</v>
+        <v>138</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>152</v>
+        <v>108</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>32</v>
@@ -4615,200 +4860,234 @@
       <c r="C67" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D67" s="1" t="s">
-        <v>311</v>
+      <c r="D67" s="5" t="s">
+        <v>306</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>160</v>
+        <v>135</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>312</v>
+        <v>41</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>110</v>
+        <v>152</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>80</v>
+        <v>41</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>315</v>
+        <v>234</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>63</v>
+        <v>160</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>64</v>
+        <v>309</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>317</v>
+        <v>234</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>209</v>
+        <v>110</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>224</v>
+        <v>312</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>207</v>
+        <v>63</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>236</v>
+        <v>314</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="D73" s="1" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>31</v>
+        <v>207</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="C74" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="D74" s="1" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>61</v>
+        <v>191</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="C75" s="1" t="s">
+        <v>167</v>
+      </c>
       <c r="D75" s="1" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>87</v>
+        <v>34</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>286</v>
+        <v>223</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B81" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C81" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D79" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>286</v>
+      <c r="D81" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>283</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Exploitation and Shelter Friends
</commit_message>
<xml_diff>
--- a/tactile_tabletop/Character Cards/Tactile_Tabletop_Data-Level_2_CC.xlsx
+++ b/tactile_tabletop/Character Cards/Tactile_Tabletop_Data-Level_2_CC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TableTopRolePlaying_Squib\tactile_tabletop\Character Cards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ofoltz\TT\TableTopRolePlaying_Squib\tactile_tabletop\Character Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7710CB86-D24D-4861-94B2-2A9729C1E7D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE975514-4767-40B6-B855-E8C6201A50A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="292" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="32190" tabRatio="292" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tactile Tabletop Data - Level 2" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="388">
   <si>
     <t>Top Ability Name</t>
   </si>
@@ -1148,6 +1148,45 @@
   </si>
   <si>
     <t>cha 16</t>
+  </si>
+  <si>
+    <t>You may play one addition cards top or bottom action in place of this action</t>
+  </si>
+  <si>
+    <t>Abuse Knowledge</t>
+  </si>
+  <si>
+    <t>You may choose the top and bottom action of one card you played this turn</t>
+  </si>
+  <si>
+    <t>Exploitation</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>1 RND</t>
+  </si>
+  <si>
+    <t>Shelter Friends</t>
+  </si>
+  <si>
+    <t>Allies</t>
+  </si>
+  <si>
+    <t>For all adjacent allies, if they take damage, instead you take that damage and reduce it by X</t>
+  </si>
+  <si>
+    <t>Healing Sap</t>
+  </si>
+  <si>
+    <t>Heal Target Ally for Y and lose X life</t>
+  </si>
+  <si>
+    <t>2 Kno</t>
+  </si>
+  <si>
+    <t>2 Vig, 1 Spi</t>
   </si>
 </sst>
 </file>
@@ -1633,10 +1672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R41"/>
+  <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="P41" sqref="P41"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3662,6 +3701,88 @@
         <v>371</v>
       </c>
     </row>
+    <row r="42" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O42" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="P42" s="1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O43" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="P43" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -3673,10 +3794,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H81"/>
+  <dimension ref="A1:I81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T31" sqref="S31:T34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3690,7 +3811,7 @@
     <col min="7" max="7" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>211</v>
       </c>
@@ -3707,7 +3828,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>91</v>
       </c>
@@ -3721,7 +3842,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>95</v>
       </c>
@@ -3738,7 +3859,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>193</v>
       </c>
@@ -3764,7 +3885,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>150</v>
       </c>
@@ -3784,7 +3905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>197</v>
       </c>
@@ -3809,8 +3930,11 @@
       <c r="H6" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>199</v>
       </c>
@@ -3833,7 +3957,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>128</v>
       </c>
@@ -3856,7 +3980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>163</v>
       </c>
@@ -3879,7 +4003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>173</v>
       </c>
@@ -3901,8 +4025,11 @@
       <c r="H10" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>142</v>
       </c>
@@ -3924,8 +4051,11 @@
       <c r="H11" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="I11" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>126</v>
       </c>
@@ -3941,7 +4071,7 @@
       </c>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>326</v>
       </c>
@@ -3959,7 +4089,7 @@
       </c>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>114</v>
       </c>
@@ -3976,7 +4106,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>187</v>
       </c>
@@ -3993,7 +4123,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>156</v>
       </c>

</xml_diff>

<commit_message>
missing column data for new cards, caused failures
</commit_message>
<xml_diff>
--- a/tactile_tabletop/Character Cards/Tactile_Tabletop_Data-Level_2_CC.xlsx
+++ b/tactile_tabletop/Character Cards/Tactile_Tabletop_Data-Level_2_CC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ofoltz\TT\TableTopRolePlaying_Squib\tactile_tabletop\Character Cards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TableTopRolePlaying_Squib\tactile_tabletop\Character Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE975514-4767-40B6-B855-E8C6201A50A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E27630-77CB-49FC-868B-F6B18D87099E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="32190" tabRatio="292" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="26370" windowHeight="15690" tabRatio="292" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tactile Tabletop Data - Level 2" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="388">
   <si>
     <t>Top Ability Name</t>
   </si>
@@ -1012,9 +1012,6 @@
     <t>Blood Trail</t>
   </si>
   <si>
-    <t>On success, target's movement is reduced by 5 ft. for X rnds. You may discard a card to mark the target as well</t>
-  </si>
-  <si>
     <t>2 Level Points</t>
   </si>
   <si>
@@ -1156,9 +1153,6 @@
     <t>Abuse Knowledge</t>
   </si>
   <si>
-    <t>You may choose the top and bottom action of one card you played this turn</t>
-  </si>
-  <si>
     <t>Exploitation</t>
   </si>
   <si>
@@ -1174,9 +1168,6 @@
     <t>Allies</t>
   </si>
   <si>
-    <t>For all adjacent allies, if they take damage, instead you take that damage and reduce it by X</t>
-  </si>
-  <si>
     <t>Healing Sap</t>
   </si>
   <si>
@@ -1187,13 +1178,41 @@
   </si>
   <si>
     <t>2 Vig, 1 Spi</t>
+  </si>
+  <si>
+    <t>For all adjacent allies, if they take damage, you take that damage instead and reduce it by X</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">You may play the top </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> bottom action of one card you played earlier this turn</t>
+    </r>
+  </si>
+  <si>
+    <t>On success, target's movement is reduced by 10 ft. for X rnds. You may discard a card to mark the target as well</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1231,6 +1250,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1674,8 +1699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1796,10 +1821,10 @@
         <v>30</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
@@ -1840,10 +1865,10 @@
         <v>30</v>
       </c>
       <c r="O3" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>330</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
@@ -1887,10 +1912,10 @@
         <v>23</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
@@ -1934,10 +1959,10 @@
         <v>23</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="51" x14ac:dyDescent="0.2">
@@ -1984,10 +2009,10 @@
         <v>30</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="89.25" x14ac:dyDescent="0.2">
@@ -2034,10 +2059,10 @@
         <v>23</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="51" x14ac:dyDescent="0.2">
@@ -2081,10 +2106,10 @@
         <v>30</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="51" x14ac:dyDescent="0.2">
@@ -2131,10 +2156,10 @@
         <v>30</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="51" x14ac:dyDescent="0.2">
@@ -2181,10 +2206,10 @@
         <v>74</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="76.5" x14ac:dyDescent="0.2">
@@ -2231,10 +2256,10 @@
         <v>23</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="63.75" x14ac:dyDescent="0.2">
@@ -2281,10 +2306,10 @@
         <v>74</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="51" x14ac:dyDescent="0.2">
@@ -2331,10 +2356,10 @@
         <v>23</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
@@ -2378,10 +2403,10 @@
         <v>30</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
@@ -2428,10 +2453,10 @@
         <v>30</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
@@ -2478,10 +2503,10 @@
         <v>30</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
@@ -2528,10 +2553,10 @@
         <v>30</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="51" x14ac:dyDescent="0.2">
@@ -2578,10 +2603,10 @@
         <v>30</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -2628,10 +2653,10 @@
         <v>23</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
@@ -2678,10 +2703,10 @@
         <v>23</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -2725,10 +2750,10 @@
         <v>30</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="51" x14ac:dyDescent="0.2">
@@ -2775,10 +2800,10 @@
         <v>23</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
@@ -2825,10 +2850,10 @@
         <v>30</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
@@ -2869,10 +2894,10 @@
         <v>30</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="51" x14ac:dyDescent="0.2">
@@ -2919,10 +2944,10 @@
         <v>23</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
@@ -2966,10 +2991,10 @@
         <v>30</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
@@ -3016,10 +3041,10 @@
         <v>30</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
@@ -3066,10 +3091,10 @@
         <v>30</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="76.5" x14ac:dyDescent="0.2">
@@ -3116,10 +3141,10 @@
         <v>30</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="51" x14ac:dyDescent="0.2">
@@ -3163,10 +3188,10 @@
         <v>23</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
@@ -3210,10 +3235,10 @@
         <v>23</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="51" x14ac:dyDescent="0.2">
@@ -3260,10 +3285,10 @@
         <v>23</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="102" x14ac:dyDescent="0.2">
@@ -3310,10 +3335,10 @@
         <v>23</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
@@ -3357,10 +3382,10 @@
         <v>30</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="89.25" x14ac:dyDescent="0.2">
@@ -3407,10 +3432,10 @@
         <v>30</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="51" x14ac:dyDescent="0.2">
@@ -3457,10 +3482,10 @@
         <v>23</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="76.5" x14ac:dyDescent="0.2">
@@ -3507,10 +3532,10 @@
         <v>23</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
@@ -3554,10 +3579,10 @@
         <v>23</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
@@ -3601,10 +3626,10 @@
         <v>23</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="51" x14ac:dyDescent="0.2">
@@ -3648,10 +3673,10 @@
         <v>23</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="51" x14ac:dyDescent="0.2">
@@ -3689,21 +3714,21 @@
         <v>44</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>329</v>
+        <v>387</v>
       </c>
       <c r="N41" s="1" t="s">
         <v>23</v>
       </c>
       <c r="O41" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>37</v>
@@ -3711,14 +3736,17 @@
       <c r="C42" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="E42" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="F42" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>37</v>
@@ -3726,40 +3754,46 @@
       <c r="J42" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="L42" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="M42" s="1" t="s">
-        <v>377</v>
+        <v>386</v>
       </c>
       <c r="N42" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O42" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="E43" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="F43" s="1" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>32</v>
@@ -3770,24 +3804,27 @@
       <c r="K43" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="L43" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="M43" s="1" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="N43" s="1" t="s">
         <v>23</v>
       </c>
       <c r="O43" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -3876,7 +3913,7 @@
         <v>220</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G4">
         <v>2</v>
@@ -3899,7 +3936,7 @@
         <v>223</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -3931,7 +3968,7 @@
         <v>227</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -3997,7 +4034,7 @@
         <v>234</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -4026,7 +4063,7 @@
         <v>227</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -4052,7 +4089,7 @@
         <v>227</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -4082,10 +4119,10 @@
         <v>19</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G13" s="1"/>
     </row>
@@ -4909,10 +4946,10 @@
         <v>44</v>
       </c>
       <c r="D62" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>369</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
-'s for ranges that don't have anything
</commit_message>
<xml_diff>
--- a/tactile_tabletop/Character Cards/Tactile_Tabletop_Data-Level_2_CC.xlsx
+++ b/tactile_tabletop/Character Cards/Tactile_Tabletop_Data-Level_2_CC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TableTopRolePlaying_Squib\tactile_tabletop\Character Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E27630-77CB-49FC-868B-F6B18D87099E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EE45B4-8FF5-4811-8BF6-45F2D7A7540A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="930" yWindow="0" windowWidth="26370" windowHeight="15690" tabRatio="292" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="387">
   <si>
     <t>Top Ability Name</t>
   </si>
@@ -86,9 +86,6 @@
     <t>Attack    X = Influence    Y = Level</t>
   </si>
   <si>
-    <t>weapon</t>
-  </si>
-  <si>
     <t>Consume an Attack Token. Make an attack against all entities within a box that is Y x Y. In addition, disperse X damage among the targets</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>Influence   X = Level</t>
   </si>
   <si>
-    <t>influence</t>
-  </si>
-  <si>
     <t>On success target reduces all rolls by X and takes X damage</t>
   </si>
   <si>
@@ -135,9 +129,6 @@
   </si>
   <si>
     <t>Self</t>
-  </si>
-  <si>
-    <t>na</t>
   </si>
   <si>
     <t>On the next instance of damage being dealt to you, instead take no damage.</t>
@@ -1206,6 +1197,12 @@
   </si>
   <si>
     <t>On success, target's movement is reduced by 10 ft. for X rnds. You may discard a card to mark the target as well</t>
+  </si>
+  <si>
+    <t>Weapon</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -1700,7 +1697,7 @@
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+      <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1791,698 +1788,695 @@
         <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="I2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="O2" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="L3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="O3" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="G4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="I4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="L4" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="N4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="I5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="L5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="N5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O5" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>329</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="I6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="L6" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="N6" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>38</v>
+        <v>386</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M8" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="O8" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M9" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="O9" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>21</v>
+        <v>385</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>21</v>
+        <v>385</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="I11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K11" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="L11" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="M11" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="N11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>38</v>
+        <v>386</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>21</v>
+        <v>385</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>21</v>
+        <v>385</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="G14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" s="1" t="s">
+      <c r="L15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M15" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="L15" s="1" t="s">
+      <c r="N15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M15" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="O15" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="H16" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>18</v>
@@ -2491,127 +2485,127 @@
         <v>19</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>21</v>
+        <v>385</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="N17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="O17" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>38</v>
+        <v>386</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>18</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>38</v>
+        <v>386</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>18</v>
@@ -2620,166 +2614,166 @@
         <v>19</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>38</v>
+        <v>386</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>38</v>
+        <v>386</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>21</v>
+        <v>385</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>21</v>
+        <v>385</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>38</v>
+        <v>386</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>21</v>
+        <v>385</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>18</v>
@@ -2788,1036 +2782,1036 @@
         <v>19</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="H23" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="L23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="N23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M23" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="O23" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>38</v>
+        <v>386</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>19</v>
       </c>
       <c r="L24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="N24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M24" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="O24" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>21</v>
+        <v>385</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>21</v>
+        <v>385</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>19</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>38</v>
+        <v>386</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="H27" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="N27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M27" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="N27" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="O27" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="M28" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>159</v>
-      </c>
       <c r="N28" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D29" s="1" t="s">
+      <c r="I29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M29" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="N29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M29" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="N29" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="O29" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="G30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J30" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D30" s="1" t="s">
+      <c r="L30" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="M30" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L30" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="N30" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M31" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L31" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M31" s="1" t="s">
-        <v>174</v>
-      </c>
       <c r="N31" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>21</v>
+        <v>385</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>21</v>
+        <v>385</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>21</v>
+        <v>385</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>21</v>
+        <v>385</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="I34" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>38</v>
+        <v>386</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>38</v>
+        <v>386</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>38</v>
+        <v>386</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="M36" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="L36" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M36" s="1" t="s">
-        <v>192</v>
-      </c>
       <c r="N36" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M37" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K37" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="L37" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M37" s="1" t="s">
-        <v>196</v>
-      </c>
       <c r="N37" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="F38" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="J38" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="G38" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H38" s="1" t="s">
+      <c r="L38" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="M38" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="I38" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="L38" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M38" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="N38" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M39" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="L39" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M39" s="1" t="s">
-        <v>206</v>
-      </c>
       <c r="N39" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E40" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F40" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="G40" s="1" t="s">
+      <c r="H40" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I40" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>19</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O41" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>38</v>
+        <v>386</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>19</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>38</v>
+        <v>386</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O42" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="43" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H43" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="G43" s="1" t="s">
+      <c r="I43" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O43" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>
@@ -3850,93 +3844,93 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="G4">
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -3944,74 +3938,74 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="G6">
         <v>2</v>
       </c>
       <c r="H6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -4019,22 +4013,22 @@
     </row>
     <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -4042,221 +4036,221 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="G11">
         <v>2</v>
       </c>
       <c r="H11" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:9" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -4270,991 +4264,991 @@
         <v>20</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F44" s="3"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="57" spans="1:6" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F57" s="3"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjusting requirements of new cards to align with the others
</commit_message>
<xml_diff>
--- a/tactile_tabletop/Character Cards/Tactile_Tabletop_Data-Level_2_CC.xlsx
+++ b/tactile_tabletop/Character Cards/Tactile_Tabletop_Data-Level_2_CC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TableTopRolePlaying_Squib\tactile_tabletop\Character Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EE45B4-8FF5-4811-8BF6-45F2D7A7540A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD5912F-D397-4E92-8D82-093DD86906F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="930" yWindow="0" windowWidth="26370" windowHeight="15690" tabRatio="292" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1163,12 +1163,6 @@
   </si>
   <si>
     <t>Heal Target Ally for Y and lose X life</t>
-  </si>
-  <si>
-    <t>2 Kno</t>
-  </si>
-  <si>
-    <t>2 Vig, 1 Spi</t>
   </si>
   <si>
     <t>For all adjacent allies, if they take damage, you take that damage instead and reduce it by X</t>
@@ -1203,6 +1197,12 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>4 Kno</t>
+  </si>
+  <si>
+    <t>1 Vig, 3 Spi</t>
   </si>
 </sst>
 </file>
@@ -1697,7 +1697,7 @@
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="L43" sqref="L43"/>
+      <selection activeCell="P43" sqref="P43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1788,7 +1788,7 @@
         <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>21</v>
@@ -1879,7 +1879,7 @@
         <v>25</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>36</v>
@@ -1900,7 +1900,7 @@
         <v>38</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>39</v>
@@ -1976,7 +1976,7 @@
         <v>46</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>47</v>
@@ -1997,7 +1997,7 @@
         <v>49</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>50</v>
@@ -2026,7 +2026,7 @@
         <v>53</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>54</v>
@@ -2047,7 +2047,7 @@
         <v>56</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>57</v>
@@ -2173,7 +2173,7 @@
         <v>46</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>68</v>
@@ -2194,7 +2194,7 @@
         <v>46</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>70</v>
@@ -2244,7 +2244,7 @@
         <v>77</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>78</v>
@@ -2273,7 +2273,7 @@
         <v>80</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>81</v>
@@ -2323,7 +2323,7 @@
         <v>20</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>85</v>
@@ -2344,7 +2344,7 @@
         <v>80</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>87</v>
@@ -2370,7 +2370,7 @@
         <v>90</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>91</v>
@@ -2417,7 +2417,7 @@
         <v>61</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>95</v>
@@ -2488,7 +2488,7 @@
         <v>103</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>104</v>
@@ -2538,7 +2538,7 @@
         <v>77</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="M17" s="1" t="s">
         <v>108</v>
@@ -2567,7 +2567,7 @@
         <v>38</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>110</v>
@@ -2588,7 +2588,7 @@
         <v>61</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>112</v>
@@ -2617,7 +2617,7 @@
         <v>41</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>114</v>
@@ -2638,7 +2638,7 @@
         <v>77</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>116</v>
@@ -2667,7 +2667,7 @@
         <v>46</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>119</v>
@@ -2688,7 +2688,7 @@
         <v>121</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="M20" s="1" t="s">
         <v>122</v>
@@ -2714,7 +2714,7 @@
         <v>19</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>124</v>
@@ -2735,7 +2735,7 @@
         <v>46</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>126</v>
@@ -2861,7 +2861,7 @@
         <v>25</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>138</v>
@@ -2908,7 +2908,7 @@
         <v>121</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>142</v>
@@ -2958,7 +2958,7 @@
         <v>121</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>146</v>
@@ -2976,7 +2976,7 @@
         <v>19</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="M26" s="1" t="s">
         <v>148</v>
@@ -3055,7 +3055,7 @@
         <v>38</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>154</v>
@@ -3076,7 +3076,7 @@
         <v>61</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="M28" s="1" t="s">
         <v>156</v>
@@ -3173,7 +3173,7 @@
         <v>25</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="M30" s="1" t="s">
         <v>167</v>
@@ -3249,7 +3249,7 @@
         <v>121</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>322</v>
@@ -3270,7 +3270,7 @@
         <v>262</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="M32" s="1" t="s">
         <v>321</v>
@@ -3299,7 +3299,7 @@
         <v>46</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>175</v>
@@ -3320,7 +3320,7 @@
         <v>260</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="M33" s="1" t="s">
         <v>177</v>
@@ -3367,7 +3367,7 @@
         <v>61</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="M34" s="1" t="s">
         <v>181</v>
@@ -3396,7 +3396,7 @@
         <v>274</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>183</v>
@@ -3417,7 +3417,7 @@
         <v>61</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="M35" s="1" t="s">
         <v>185</v>
@@ -3446,7 +3446,7 @@
         <v>61</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>187</v>
@@ -3467,7 +3467,7 @@
         <v>164</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="M36" s="1" t="s">
         <v>189</v>
@@ -3564,7 +3564,7 @@
         <v>198</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="M38" s="1" t="s">
         <v>199</v>
@@ -3708,7 +3708,7 @@
         <v>41</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="N41" s="1" t="s">
         <v>22</v>
@@ -3731,7 +3731,7 @@
         <v>19</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>371</v>
@@ -3749,10 +3749,10 @@
         <v>19</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N42" s="1" t="s">
         <v>28</v>
@@ -3761,7 +3761,7 @@
         <v>326</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>380</v>
+        <v>385</v>
       </c>
     </row>
     <row r="43" spans="1:16" ht="51" x14ac:dyDescent="0.2">
@@ -3778,10 +3778,10 @@
         <v>38</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>28</v>
@@ -3811,7 +3811,7 @@
         <v>326</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>381</v>
+        <v>386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>